<commit_message>
Updation of quick quote
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/QA_517.xlsx
+++ b/binaries/FCfiles/QA_517.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="105">
   <si>
     <t>shipmentType</t>
   </si>
@@ -329,6 +329,18 @@
   </si>
   <si>
     <t>51498315</t>
+  </si>
+  <si>
+    <t>51498469</t>
+  </si>
+  <si>
+    <t>51498470</t>
+  </si>
+  <si>
+    <t>51498471</t>
+  </si>
+  <si>
+    <t>51498472</t>
   </si>
 </sst>
 </file>
@@ -365,7 +377,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="50">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -572,8 +584,48 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="40">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -776,12 +828,40 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -818,7 +898,11 @@
     <xf applyBorder="true" applyFill="true" borderId="33" fillId="35" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="35" fillId="37" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="37" fillId="39" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="39" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="39" fillId="41" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="41" fillId="43" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="43" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="45" fillId="47" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="47" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1400,8 +1484,8 @@
       <c r="Q2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="33" t="s">
-        <v>97</v>
+      <c r="R2" s="37" t="s">
+        <v>101</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>79</v>
@@ -1463,8 +1547,8 @@
       <c r="Q3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="34" t="s">
-        <v>98</v>
+      <c r="R3" s="38" t="s">
+        <v>102</v>
       </c>
       <c r="S3" s="9" t="s">
         <v>80</v>
@@ -1526,8 +1610,8 @@
       <c r="Q4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R4" s="35" t="s">
-        <v>99</v>
+      <c r="R4" s="39" t="s">
+        <v>103</v>
       </c>
       <c r="S4" s="9" t="s">
         <v>80</v>
@@ -1589,8 +1673,8 @@
       <c r="Q5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="36" t="s">
-        <v>100</v>
+      <c r="R5" s="40" t="s">
+        <v>104</v>
       </c>
       <c r="S5" s="9" t="s">
         <v>80</v>

</xml_diff>